<commit_message>
Habilitar a entrada de dados
Habilitar a entrada de dados
</commit_message>
<xml_diff>
--- a/Datasource/Results/scoop-A_AP-9.d_3_RandonShuffle.xlsx
+++ b/Datasource/Results/scoop-A_AP-9.d_3_RandonShuffle.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B482"/>
+  <dimension ref="A1:B486"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4226,6 +4226,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="483">
+      <c r="A483" t="n">
+        <v>11</v>
+      </c>
+      <c r="B483" t="n">
+        <v>0.000977</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n">
+        <v>13</v>
+      </c>
+      <c r="B484" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="n">
+        <v>11</v>
+      </c>
+      <c r="B485" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n">
+        <v>13</v>
+      </c>
+      <c r="B486" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>